<commit_message>
correct conneXion.xlsx and AISA.xlsx
</commit_message>
<xml_diff>
--- a/runtime/apps/AISA/AISA.xlsx
+++ b/runtime/apps/AISA/AISA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\athena\github\trusted-service\runtime\apps\AISA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3246593C-4A06-4B23-9612-57C25BF4E452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0612BF-02AE-4B34-BC72-ED76A108D113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="973" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="973" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="APP &amp; MODEL" sheetId="25" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="136">
   <si>
     <t>Parameter</t>
   </si>
@@ -69,30 +69,9 @@
     <t>str</t>
   </si>
   <si>
-    <t>bool</t>
-  </si>
-  <si>
     <t># Does not support formulas</t>
   </si>
   <si>
-    <t>AES</t>
-  </si>
-  <si>
-    <t>ANEF (Administration Numérique pour les Etrangers en France)</t>
-  </si>
-  <si>
-    <t>La plateforme permettant aux usagers de réaliser un certain nombre de démarches : Validation du Visa Long Séjour valant Titre de Séjour,  Demandes concernant certains titres de séjour,  Demande de documents de voyage,  Demande de naturalisation,  Demande d'autorisation de travail,  Changement d'adresse.</t>
-  </si>
-  <si>
-    <t>API</t>
-  </si>
-  <si>
-    <t>ATDA</t>
-  </si>
-  <si>
-    <t>DCEM</t>
-  </si>
-  <si>
     <t>term</t>
   </si>
   <si>
@@ -114,9 +93,6 @@
     <t>DO NOT EXTRACT</t>
   </si>
   <si>
-    <t>EXTRACT AND HIGHLIGHT</t>
-  </si>
-  <si>
     <t>send_to_decision_engine</t>
   </si>
   <si>
@@ -237,30 +213,6 @@
     <t>Email address</t>
   </si>
   <si>
-    <t>Admission Exceptionnelle au Séjour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attestation de Prolongation de l’Instruction, document généré depuis la plateforme ANEF </t>
-  </si>
-  <si>
-    <t>ATtestation de Demande d’Asile</t>
-  </si>
-  <si>
-    <t>Document de Circulation pour Etranger Mineur</t>
-  </si>
-  <si>
-    <t>Admission Exceptionnelle au Séjour (Exceptional Admission to Residence)</t>
-  </si>
-  <si>
-    <t>The platform that allows users to carry out a number of procedures: validation of a Long-Stay Visa serving as a Residence Permit, applications concerning certain residence permits, application for travel documents, application for naturalisation, application for work authorisation, and change of address</t>
-  </si>
-  <si>
-    <t>Attestation de Prolongation de l’Instruction (Certificate of Extension of Processing, a document generated from the ANEF platform)</t>
-  </si>
-  <si>
-    <t>Document de Circulation pour Etranger Mineur (Travel Document for a Minor Foreigner)</t>
-  </si>
-  <si>
     <t>app_name_en</t>
   </si>
   <si>
@@ -306,9 +258,6 @@
     <t>Veuillez consulter la page [{0}]({1})</t>
   </si>
   <si>
-    <t>Attestation de Demande d’Asile (Certificate of Asylum Application)</t>
-  </si>
-  <si>
     <t>True</t>
   </si>
   <si>
@@ -348,9 +297,6 @@
     <t>Date of the message (DD/MM/YYYY)</t>
   </si>
   <si>
-    <t>plan</t>
-  </si>
-  <si>
     <t>Unlimited Data Plans</t>
   </si>
   <si>
@@ -390,12 +336,6 @@
     <t>speed_based_plans</t>
   </si>
   <si>
-    <t>Data plan</t>
-  </si>
-  <si>
-    <t>plans</t>
-  </si>
-  <si>
     <t>surname</t>
   </si>
   <si>
@@ -403,15 +343,6 @@
   </si>
   <si>
     <t>email_address</t>
-  </si>
-  <si>
-    <t>billing_issues</t>
-  </si>
-  <si>
-    <t>Have you recently changed your plan or added any services?</t>
-  </si>
-  <si>
-    <t>recently_changed_plan_or_added_services</t>
   </si>
   <si>
     <t>Today is {date_message} (DD/MM/YYYY).  
@@ -424,30 +355,12 @@
     <t>Client is expressing some frustration</t>
   </si>
   <si>
-    <t>level_of_frustration</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The level of frustration between 1 (Not frustrated at all) and 5 (Critically frustrated) </t>
-  </si>
-  <si>
-    <t>customer_lifetime_value</t>
-  </si>
-  <si>
-    <t>Customer Lifetime Value (Low, Medium, High)</t>
-  </si>
-  <si>
     <t>CLIENT_HIGH_VALUE</t>
   </si>
   <si>
     <t>High value client</t>
   </si>
   <si>
-    <t>Level of frustration (1 to 5)</t>
-  </si>
-  <si>
     <t>parameter1</t>
   </si>
   <si>
@@ -472,12 +385,6 @@
     <t>do not rename as it is the default value for v1 legacy calls</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>runtime.apps.conneXion.decision_engine</t>
-  </si>
-  <si>
     <t>DecisionEngineConnexion</t>
   </si>
   <si>
@@ -538,9 +445,24 @@
     <t>control_of_plots_rented_by_the_city_and_management_of_vacant_plots</t>
   </si>
   <si>
+    <t>district</t>
+  </si>
+  <si>
+    <t>In what district</t>
+  </si>
+  <si>
+    <t>Helsink center</t>
+  </si>
+  <si>
     <t>Dear city of Helsinki building services,
-I am writing to you regarding city plots for an apartment block &amp; a terraced building.
-Please let me know.</t>
+I am interested in acquiring building plots for both building a new gym and a restaurant.
+Please let me know how to proceed.</t>
+  </si>
+  <si>
+    <t>runtime.apps.AISA.decision_engine</t>
+  </si>
+  <si>
+    <t>city_plots_for_apartment_blocks_and_terraced_houses complimentary_construction_for_housing_cooperative_plots</t>
   </si>
 </sst>
 </file>
@@ -563,15 +485,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF040C28"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -629,17 +552,14 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
@@ -654,9 +574,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
@@ -665,9 +585,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -969,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40884519-E9E2-4702-AA20-B46B229B9942}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,105 +909,105 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>51</v>
+      <c r="B5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>147</v>
+      <c r="A6" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>148</v>
+      <c r="A7" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>149</v>
+      <c r="A8" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>150</v>
+      <c r="A9" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>151</v>
+      <c r="A10" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>152</v>
+      <c r="A11" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>153</v>
+      <c r="A12" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1121,7 +1048,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1134,43 +1061,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="F1" s="6" t="s">
+      <c r="B1" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>140</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>90</v>
+        <v>110</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>73</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>138</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1210,79 +1137,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="5"/>
+      <c r="A2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="5"/>
+      <c r="A3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="5"/>
+      <c r="A4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="5"/>
+      <c r="A5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="5"/>
+      <c r="A6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="5">
+      <c r="A7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="4">
         <v>587</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>71</v>
+      <c r="A8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1310,20 +1237,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>25</v>
+      <c r="B1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1366,108 +1293,108 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="B7" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C4" s="8" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="F5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>105</v>
+      <c r="C8" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>105</v>
+      <c r="A9" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1491,33 +1418,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="5"/>
+      <c r="A2" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="C3" s="5"/>
+      <c r="A3" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1540,51 +1467,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="5"/>
+      <c r="A2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="C3" s="5"/>
+      <c r="A3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>70</v>
+      <c r="A4" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C4" s="5"/>
+        <v>115</v>
+      </c>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>94</v>
+      <c r="A5" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C5" s="5"/>
+        <v>133</v>
+      </c>
+      <c r="C5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1607,27 +1534,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>74</v>
+      <c r="A1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>129</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1652,43 +1579,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>80</v>
+      <c r="A1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1698,10 +1625,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF16B1B1-A6B4-4B56-9813-CCF1B731EDAC}">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1716,406 +1643,274 @@
     <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.140625" customWidth="1"/>
-    <col min="11" max="11" width="58" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="108.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="77" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="B1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="H1" s="4" t="s">
+      <c r="M1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="I4" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="K2" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="L2" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="B3" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="K3" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="L3" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="K4" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="L4" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="K5" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="L5" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>86</v>
+      <c r="C5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="I6" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="K6" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="L6" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="L7" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="M7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="N7" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="K8" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="M8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="N8" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="K9" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="L9" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="N9" s="8" t="s">
-        <v>85</v>
+      <c r="J6" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="K6" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="L6" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="M6" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="N6" s="18" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2149,7 +1944,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2161,24 +1956,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>55</v>
+      <c r="A2" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C2" s="5"/>
+        <v>97</v>
+      </c>
+      <c r="C2" s="4"/>
     </row>
     <row r="4" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2198,10 +1993,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F212B83-BB31-486E-8D1E-C153171C389E}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2212,69 +2007,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete Finnish localization for use case 1
</commit_message>
<xml_diff>
--- a/runtime/apps/AISA/AISA.xlsx
+++ b/runtime/apps/AISA/AISA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\athena\github\trusted-service\runtime\apps\AISA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F47AFA-2EFB-4CB8-B28A-AF487966C995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4829A5-1448-4B4C-BFAA-F2F2C6FA1E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="0" windowWidth="14565" windowHeight="15480" tabRatio="973" firstSheet="11" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-360" yWindow="0" windowWidth="15465" windowHeight="15480" tabRatio="973" firstSheet="7" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="APP &amp; MODEL" sheetId="25" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="346">
   <si>
     <t>Parameter</t>
   </si>
@@ -437,21 +437,6 @@
   </si>
   <si>
     <t>label_sv</t>
-  </si>
-  <si>
-    <t>010-kruununhaka</t>
-  </si>
-  <si>
-    <t>020-kluuvi</t>
-  </si>
-  <si>
-    <t>080-katajanokka</t>
-  </si>
-  <si>
-    <t>1-eteläinen_suurpiiri</t>
-  </si>
-  <si>
-    <t>101-vironniemen_peruspiiri</t>
   </si>
   <si>
     <t>districts</t>
@@ -561,6 +546,562 @@
   </si>
   <si>
     <t>Kaupungin vuokraamien tonttien valvonta ja tyhjien tonttien isännöinti</t>
+  </si>
+  <si>
+    <t>1-kruununhaka</t>
+  </si>
+  <si>
+    <t>1 Kruununhaka</t>
+  </si>
+  <si>
+    <t>Kronhagen</t>
+  </si>
+  <si>
+    <t>2-kluuvi</t>
+  </si>
+  <si>
+    <t>2 Kluuvi</t>
+  </si>
+  <si>
+    <t>Gloet</t>
+  </si>
+  <si>
+    <t>3-kaartinkaupunki</t>
+  </si>
+  <si>
+    <t>3 Kaartinkaupunki</t>
+  </si>
+  <si>
+    <t>Gardesstaden</t>
+  </si>
+  <si>
+    <t>4-kamppi</t>
+  </si>
+  <si>
+    <t>4 Kamppi</t>
+  </si>
+  <si>
+    <t>Kampen</t>
+  </si>
+  <si>
+    <t>5-punavuori</t>
+  </si>
+  <si>
+    <t>5 Punavuori</t>
+  </si>
+  <si>
+    <t>Rödbergen</t>
+  </si>
+  <si>
+    <t>6-eira</t>
+  </si>
+  <si>
+    <t>6 Eira</t>
+  </si>
+  <si>
+    <t>Eira</t>
+  </si>
+  <si>
+    <t>7-ullanlinna</t>
+  </si>
+  <si>
+    <t>07 Ullanlinna</t>
+  </si>
+  <si>
+    <t>Ulrikasborg</t>
+  </si>
+  <si>
+    <t>8-katajanokka</t>
+  </si>
+  <si>
+    <t>08 Katajanokka</t>
+  </si>
+  <si>
+    <t>Skatudden</t>
+  </si>
+  <si>
+    <t>9-kaivopuisto</t>
+  </si>
+  <si>
+    <t>09 Kaivopuisto</t>
+  </si>
+  <si>
+    <t>Brunnsparken</t>
+  </si>
+  <si>
+    <t>10-sornäinen</t>
+  </si>
+  <si>
+    <t>10 Sörnäinen</t>
+  </si>
+  <si>
+    <t>Sörnäs</t>
+  </si>
+  <si>
+    <t>11-kallio</t>
+  </si>
+  <si>
+    <t>11 Kallio</t>
+  </si>
+  <si>
+    <t>Berghäll</t>
+  </si>
+  <si>
+    <t>12-alppiharju</t>
+  </si>
+  <si>
+    <t>12 Alppiharju</t>
+  </si>
+  <si>
+    <t>Åshöjden</t>
+  </si>
+  <si>
+    <t>13-etu-toolo</t>
+  </si>
+  <si>
+    <t>13 Etu-Töölö</t>
+  </si>
+  <si>
+    <t>Främre Tölö</t>
+  </si>
+  <si>
+    <t>14-taka-toolo</t>
+  </si>
+  <si>
+    <t>14 Taka-Töölö</t>
+  </si>
+  <si>
+    <t>Bortre Tölö</t>
+  </si>
+  <si>
+    <t>15-meilahti</t>
+  </si>
+  <si>
+    <t>15 Meilahti</t>
+  </si>
+  <si>
+    <t>Mejlans</t>
+  </si>
+  <si>
+    <t>16-ruskeasuo</t>
+  </si>
+  <si>
+    <t>16 Ruskeasuo</t>
+  </si>
+  <si>
+    <t>Brunakärr</t>
+  </si>
+  <si>
+    <t>17-pasila</t>
+  </si>
+  <si>
+    <t>17 Pasila</t>
+  </si>
+  <si>
+    <t>Böle</t>
+  </si>
+  <si>
+    <t>18-laakso</t>
+  </si>
+  <si>
+    <t>18 Laakso</t>
+  </si>
+  <si>
+    <t>Dal</t>
+  </si>
+  <si>
+    <t>19-mustikkamaa-korkeasaari</t>
+  </si>
+  <si>
+    <t>19 Mustikkamaa-Korkeasaari</t>
+  </si>
+  <si>
+    <t>Blåbärslandet-Högholmen</t>
+  </si>
+  <si>
+    <t>20-lansisatama</t>
+  </si>
+  <si>
+    <t>20 Länsisatama</t>
+  </si>
+  <si>
+    <t>Västra hamnen</t>
+  </si>
+  <si>
+    <t>21-hermanni</t>
+  </si>
+  <si>
+    <t>21 Hermanni</t>
+  </si>
+  <si>
+    <t>Hermanstad</t>
+  </si>
+  <si>
+    <t>22-vallila</t>
+  </si>
+  <si>
+    <t>22 Vallila</t>
+  </si>
+  <si>
+    <t>Vallgård</t>
+  </si>
+  <si>
+    <t>23-toukola</t>
+  </si>
+  <si>
+    <t>23 Toukola</t>
+  </si>
+  <si>
+    <t>Majstad</t>
+  </si>
+  <si>
+    <t>24-kumpula</t>
+  </si>
+  <si>
+    <t>24 Kumpula</t>
+  </si>
+  <si>
+    <t>Gumtäkt</t>
+  </si>
+  <si>
+    <t>25-kapyla</t>
+  </si>
+  <si>
+    <t>25 Käpylä</t>
+  </si>
+  <si>
+    <t>Kottby</t>
+  </si>
+  <si>
+    <t>26-koskela</t>
+  </si>
+  <si>
+    <t>26 Koskela</t>
+  </si>
+  <si>
+    <t>Forsby</t>
+  </si>
+  <si>
+    <t>27-vanhakaupunki</t>
+  </si>
+  <si>
+    <t>27 Vanhakaupunki</t>
+  </si>
+  <si>
+    <t>Gammelstaden</t>
+  </si>
+  <si>
+    <t>28-oulunkyla</t>
+  </si>
+  <si>
+    <t>28 Oulunkylä</t>
+  </si>
+  <si>
+    <t>Åggelby</t>
+  </si>
+  <si>
+    <t>29-haaga</t>
+  </si>
+  <si>
+    <t>29 Haaga</t>
+  </si>
+  <si>
+    <t>Haga</t>
+  </si>
+  <si>
+    <t>30-munkkiniemi</t>
+  </si>
+  <si>
+    <t>30 Munkkiniemi</t>
+  </si>
+  <si>
+    <t>Munksnäs</t>
+  </si>
+  <si>
+    <t>31-lauttasaari</t>
+  </si>
+  <si>
+    <t>31 Lauttasaari</t>
+  </si>
+  <si>
+    <t>Drumsö</t>
+  </si>
+  <si>
+    <t>32-konala</t>
+  </si>
+  <si>
+    <t>32 Konala</t>
+  </si>
+  <si>
+    <t>Kånala</t>
+  </si>
+  <si>
+    <t>33-kaarela</t>
+  </si>
+  <si>
+    <t>33 Kaarela</t>
+  </si>
+  <si>
+    <t>Kårböle</t>
+  </si>
+  <si>
+    <t>34-pakila</t>
+  </si>
+  <si>
+    <t>34 Pakila</t>
+  </si>
+  <si>
+    <t>Baggböle</t>
+  </si>
+  <si>
+    <t>35-tuomarinkyla</t>
+  </si>
+  <si>
+    <t>35 Tuomarinkylä</t>
+  </si>
+  <si>
+    <t>Domarby</t>
+  </si>
+  <si>
+    <t>36-viikki</t>
+  </si>
+  <si>
+    <t>36 Viikki</t>
+  </si>
+  <si>
+    <t>Vik</t>
+  </si>
+  <si>
+    <t>37-pukinmaki</t>
+  </si>
+  <si>
+    <t>37 Pukinmäki</t>
+  </si>
+  <si>
+    <t>Bocksbacka</t>
+  </si>
+  <si>
+    <t>38-malmi</t>
+  </si>
+  <si>
+    <t>38 Malmi</t>
+  </si>
+  <si>
+    <t>Malm</t>
+  </si>
+  <si>
+    <t>39-tapaninkyla</t>
+  </si>
+  <si>
+    <t>39 Tapaninkylä</t>
+  </si>
+  <si>
+    <t>Staffansby</t>
+  </si>
+  <si>
+    <t>40-suutarila</t>
+  </si>
+  <si>
+    <t>40 Suutarila</t>
+  </si>
+  <si>
+    <t>Skomakarböle</t>
+  </si>
+  <si>
+    <t>41-suurmetsa</t>
+  </si>
+  <si>
+    <t>41 Suurmetsä</t>
+  </si>
+  <si>
+    <t>Storskog</t>
+  </si>
+  <si>
+    <t>42-kulosaari</t>
+  </si>
+  <si>
+    <t>42 Kulosaari</t>
+  </si>
+  <si>
+    <t>Brändö</t>
+  </si>
+  <si>
+    <t>43-herttoniemi</t>
+  </si>
+  <si>
+    <t>43 Herttoniemi</t>
+  </si>
+  <si>
+    <t>Hertonäs</t>
+  </si>
+  <si>
+    <t>44-tammisalo</t>
+  </si>
+  <si>
+    <t>44 Tammisalo</t>
+  </si>
+  <si>
+    <t>Tammelund</t>
+  </si>
+  <si>
+    <t>45-vartiokyla</t>
+  </si>
+  <si>
+    <t>45 Vartiokylä</t>
+  </si>
+  <si>
+    <t>Botby</t>
+  </si>
+  <si>
+    <t>46-pitajanmaki</t>
+  </si>
+  <si>
+    <t>46 Pitäjänmäki</t>
+  </si>
+  <si>
+    <t>Sockenbacka</t>
+  </si>
+  <si>
+    <t>47-mellunkyla</t>
+  </si>
+  <si>
+    <t>47 Mellunkylä</t>
+  </si>
+  <si>
+    <t>Mellungsby</t>
+  </si>
+  <si>
+    <t>48-vartiosaari</t>
+  </si>
+  <si>
+    <t>48 Vartiosaari</t>
+  </si>
+  <si>
+    <t>Vårdö</t>
+  </si>
+  <si>
+    <t>49-laajasalo</t>
+  </si>
+  <si>
+    <t>49 Laajasalo</t>
+  </si>
+  <si>
+    <t>Degerö</t>
+  </si>
+  <si>
+    <t>50-villinki</t>
+  </si>
+  <si>
+    <t>50 Villinki</t>
+  </si>
+  <si>
+    <t>Villinge</t>
+  </si>
+  <si>
+    <t>51-santahamina</t>
+  </si>
+  <si>
+    <t>51 Santahamina</t>
+  </si>
+  <si>
+    <t>Sandhamn</t>
+  </si>
+  <si>
+    <t>52-suomenlinna</t>
+  </si>
+  <si>
+    <t>52 Suomenlinna</t>
+  </si>
+  <si>
+    <t>Sveaborg</t>
+  </si>
+  <si>
+    <t>53-ulkosaaret</t>
+  </si>
+  <si>
+    <t>53 Ulkosaaret</t>
+  </si>
+  <si>
+    <t>Utöarna</t>
+  </si>
+  <si>
+    <t>54-vuosaari</t>
+  </si>
+  <si>
+    <t>54 Vuosaari</t>
+  </si>
+  <si>
+    <t>Nordsjö</t>
+  </si>
+  <si>
+    <t>55-ostersundom</t>
+  </si>
+  <si>
+    <t>55 Östersundom</t>
+  </si>
+  <si>
+    <t>Östersundom</t>
+  </si>
+  <si>
+    <t>56-salmenkallio</t>
+  </si>
+  <si>
+    <t>56 Salmenkallio</t>
+  </si>
+  <si>
+    <t>Sundberg</t>
+  </si>
+  <si>
+    <t>57-talosaari</t>
+  </si>
+  <si>
+    <t>57 Talosaari</t>
+  </si>
+  <si>
+    <t>Husö</t>
+  </si>
+  <si>
+    <t>58-karhusaari</t>
+  </si>
+  <si>
+    <t>58 Karhusaari</t>
+  </si>
+  <si>
+    <t>Björnsö</t>
+  </si>
+  <si>
+    <t>59-ultuna</t>
+  </si>
+  <si>
+    <t>59 Ultuna</t>
+  </si>
+  <si>
+    <t>Ultuna</t>
+  </si>
+  <si>
+    <t>aluemeri</t>
+  </si>
+  <si>
+    <t>Aluemeri</t>
+  </si>
+  <si>
+    <t>Territorialhavet</t>
+  </si>
+  <si>
+    <t>Kysymyksesi on välitetty eteenpäin käsittelyä varten.</t>
+  </si>
+  <si>
+    <t>Katso lisätietoa: [{0}]({1})</t>
+  </si>
+  <si>
+    <t>Esimerkki: nimi@esimerkki.com</t>
+  </si>
+  <si>
+    <t>https://www.hel.fi/fi/kaupunkiymparisto-ja-liikenne/tontit-ja-rakentamisen-luvat/yhteystiedot-rakennusvalvonta-tontit-ja-lupa-asiat#tonttipalvelujen-yhteystiedot-kartalla</t>
+  </si>
+  <si>
+    <t>Tänään on {date_message} (DD/MM/YYYY).  
+Olet asiakaspalvelija, joka arvioi ja ohjaa kyselyjä eteenpäin asiakaspalvelutiimeille.</t>
   </si>
 </sst>
 </file>
@@ -610,7 +1151,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -631,6 +1172,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -664,7 +1211,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -708,18 +1255,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="2" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1022,7 +1564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40884519-E9E2-4702-AA20-B46B229B9942}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -1062,13 +1604,13 @@
         <v>126</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>127</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1081,11 +1623,11 @@
       <c r="C6" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D6" s="29" t="s">
-        <v>159</v>
-      </c>
-      <c r="E6" s="29" t="s">
-        <v>159</v>
+      <c r="D6" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>154</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>97</v>
@@ -1104,11 +1646,11 @@
       <c r="C7" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D7" s="29" t="s">
-        <v>160</v>
-      </c>
-      <c r="E7" s="29" t="s">
-        <v>160</v>
+      <c r="D7" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>155</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>98</v>
@@ -1127,11 +1669,11 @@
       <c r="C8" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D8" s="29" t="s">
-        <v>161</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>161</v>
+      <c r="D8" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>99</v>
@@ -1150,11 +1692,11 @@
       <c r="C9" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D9" s="29" t="s">
-        <v>162</v>
-      </c>
-      <c r="E9" s="29" t="s">
-        <v>162</v>
+      <c r="D9" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>157</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>100</v>
@@ -1173,11 +1715,11 @@
       <c r="C10" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="D10" s="29" t="s">
-        <v>163</v>
-      </c>
-      <c r="E10" s="29" t="s">
-        <v>163</v>
+      <c r="D10" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>158</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>101</v>
@@ -1196,11 +1738,11 @@
       <c r="C11" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="D11" s="29" t="s">
-        <v>164</v>
-      </c>
-      <c r="E11" s="29" t="s">
-        <v>164</v>
+      <c r="D11" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>159</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>102</v>
@@ -1219,11 +1761,11 @@
       <c r="C12" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="D12" s="29" t="s">
-        <v>165</v>
-      </c>
-      <c r="E12" s="29" t="s">
-        <v>165</v>
+      <c r="D12" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>160</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>103</v>
@@ -1277,7 +1819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5609F2C9-1DAC-445D-8758-7844C0303FDB}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1355,8 +1897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD020DE-44B7-44EF-BEA3-8491F2595E0A}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1507,10 +2049,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48C25835-C93B-43AA-B5BF-FF69903103A9}">
-  <dimension ref="A1:R31"/>
+  <dimension ref="A1:R63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1555,21 +2097,21 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>131</v>
+        <v>161</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>116</v>
+        <v>162</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>116</v>
+        <v>162</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>78</v>
       </c>
       <c r="I4" s="17"/>
@@ -1582,21 +2124,21 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>132</v>
+        <v>164</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>118</v>
+        <v>165</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>118</v>
+        <v>165</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="F5" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>78</v>
       </c>
       <c r="I5" s="17"/>
@@ -1609,21 +2151,21 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>128</v>
+        <v>167</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>120</v>
+        <v>168</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>120</v>
+        <v>168</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="F6" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>78</v>
       </c>
       <c r="I6" s="17"/>
@@ -1636,21 +2178,21 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>129</v>
+        <v>170</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>122</v>
+        <v>171</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>122</v>
+        <v>171</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="F7" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>78</v>
       </c>
       <c r="I7" s="17"/>
@@ -1663,21 +2205,21 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>130</v>
+        <v>173</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>124</v>
+        <v>174</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>124</v>
+        <v>174</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>78</v>
       </c>
       <c r="I8" s="17"/>
@@ -1688,10 +2230,1220 @@
         <v>125</v>
       </c>
     </row>
-    <row r="31" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>78</v>
+      </c>
       <c r="I31" s="16"/>
     </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C9" r:id="rId1" tooltip="Eira" display="https://fi.wikipedia.org/wiki/Eira" xr:uid="{81217712-9232-4AEC-8C59-88D11443F81E}"/>
+    <hyperlink ref="C10" r:id="rId2" tooltip="Ullanlinna" display="https://fi.wikipedia.org/wiki/Ullanlinna" xr:uid="{E01A95F0-3A9C-4151-BB43-226E58DFBC76}"/>
+    <hyperlink ref="C11" r:id="rId3" tooltip="Katajanokka" display="https://fi.wikipedia.org/wiki/Katajanokka" xr:uid="{40F90D74-70B6-46A9-8BA3-58FC5F6739DE}"/>
+    <hyperlink ref="C12" r:id="rId4" tooltip="Kaivopuisto" display="https://fi.wikipedia.org/wiki/Kaivopuisto" xr:uid="{A55F337C-B289-4DBE-B6EA-D2F33CD41490}"/>
+    <hyperlink ref="C13" r:id="rId5" tooltip="Sörnäinen" display="https://fi.wikipedia.org/wiki/S%C3%B6rn%C3%A4inen" xr:uid="{E7F6640D-BB8A-4427-B498-A62085F422EC}"/>
+    <hyperlink ref="C14" r:id="rId6" tooltip="Kallio (Helsinki)" display="https://fi.wikipedia.org/wiki/Kallio_(Helsinki)" xr:uid="{CE487E00-AD7F-430C-9D16-4B2896A6E8B1}"/>
+    <hyperlink ref="C15" r:id="rId7" tooltip="Alppiharju" display="https://fi.wikipedia.org/wiki/Alppiharju" xr:uid="{029D4408-7795-4300-B55F-0A01A4203FFD}"/>
+    <hyperlink ref="C16" r:id="rId8" tooltip="Etu-Töölö" display="https://fi.wikipedia.org/wiki/Etu-T%C3%B6%C3%B6l%C3%B6" xr:uid="{1B7F507A-75A8-4257-978F-3222286C50BF}"/>
+    <hyperlink ref="C17" r:id="rId9" tooltip="Taka-Töölö" display="https://fi.wikipedia.org/wiki/Taka-T%C3%B6%C3%B6l%C3%B6" xr:uid="{FEDF3153-190D-4E46-9D93-34E3DFEF297B}"/>
+    <hyperlink ref="C18" r:id="rId10" tooltip="Meilahti" display="https://fi.wikipedia.org/wiki/Meilahti" xr:uid="{F370CC79-D059-4DCD-9D63-25AF58015EF8}"/>
+    <hyperlink ref="C19" r:id="rId11" tooltip="Ruskeasuo" display="https://fi.wikipedia.org/wiki/Ruskeasuo" xr:uid="{B63F032C-A107-4F6E-80D1-6344585F5AC2}"/>
+    <hyperlink ref="C20" r:id="rId12" tooltip="Pasila" display="https://fi.wikipedia.org/wiki/Pasila" xr:uid="{235F9129-C90B-4F0B-A536-4F7471FE9EFC}"/>
+    <hyperlink ref="C21" r:id="rId13" tooltip="Laakso (Helsinki)" display="https://fi.wikipedia.org/wiki/Laakso_(Helsinki)" xr:uid="{75890470-2ED3-4C37-A88E-BFCEB84F3688}"/>
+    <hyperlink ref="C22" r:id="rId14" tooltip="Mustikkamaa-Korkeasaari" display="https://fi.wikipedia.org/wiki/Mustikkamaa-Korkeasaari" xr:uid="{C7EF8458-BF4E-4245-A03D-81D87190E0E0}"/>
+    <hyperlink ref="C23" r:id="rId15" tooltip="Länsisatama (Helsinki)" display="https://fi.wikipedia.org/wiki/L%C3%A4nsisatama_(Helsinki)" xr:uid="{46CDD662-6320-4DF6-9E5B-9B8DB4A58C25}"/>
+    <hyperlink ref="C24" r:id="rId16" tooltip="Hermanni (Helsinki)" display="https://fi.wikipedia.org/wiki/Hermanni_(Helsinki)" xr:uid="{4F33DF46-5EB5-4112-A1DF-6D9B46FAF170}"/>
+    <hyperlink ref="C25" r:id="rId17" tooltip="Vallila" display="https://fi.wikipedia.org/wiki/Vallila" xr:uid="{F7F82D59-B7DA-4134-AFDD-232BE6800CB8}"/>
+    <hyperlink ref="C26" r:id="rId18" tooltip="Toukola" display="https://fi.wikipedia.org/wiki/Toukola" xr:uid="{E74F6141-B314-4632-95C4-7545CC45631B}"/>
+    <hyperlink ref="C27" r:id="rId19" tooltip="Kumpula" display="https://fi.wikipedia.org/wiki/Kumpula" xr:uid="{58AE53E7-C12D-4269-A101-869923BF474A}"/>
+    <hyperlink ref="C28" r:id="rId20" tooltip="Käpylä" display="https://fi.wikipedia.org/wiki/K%C3%A4pyl%C3%A4" xr:uid="{008C67EC-5D50-4606-8305-D15C77134272}"/>
+    <hyperlink ref="C29" r:id="rId21" tooltip="Koskela (Helsinki)" display="https://fi.wikipedia.org/wiki/Koskela_(Helsinki)" xr:uid="{E1E9655F-6355-4120-B7A0-7F2B4FF7218C}"/>
+    <hyperlink ref="C30" r:id="rId22" tooltip="Vanhakaupunki (Helsinki)" display="https://fi.wikipedia.org/wiki/Vanhakaupunki_(Helsinki)" xr:uid="{9EF6FCE9-F37E-4554-8B86-F8D92364CAFC}"/>
+    <hyperlink ref="C31" r:id="rId23" tooltip="Oulunkylä" display="https://fi.wikipedia.org/wiki/Oulunkyl%C3%A4" xr:uid="{BE29CCB2-B57D-4645-923D-61C6E283D1D0}"/>
+    <hyperlink ref="C32" r:id="rId24" tooltip="Haaga" display="https://fi.wikipedia.org/wiki/Haaga" xr:uid="{E8980AD0-9152-4545-80DC-BB68D943048A}"/>
+    <hyperlink ref="C33" r:id="rId25" tooltip="Munkkiniemi" display="https://fi.wikipedia.org/wiki/Munkkiniemi" xr:uid="{0BFB63BA-F4BA-4C7C-9DDC-8F820EBB91E9}"/>
+    <hyperlink ref="C34" r:id="rId26" tooltip="Lauttasaari" display="https://fi.wikipedia.org/wiki/Lauttasaari" xr:uid="{957CA2A8-3943-4A75-8C16-BAB3D9E9E705}"/>
+    <hyperlink ref="C35" r:id="rId27" tooltip="Konala" display="https://fi.wikipedia.org/wiki/Konala" xr:uid="{0FE0C0D3-AFDC-4B59-856D-4F4811DA83AC}"/>
+    <hyperlink ref="C36" r:id="rId28" tooltip="Kaarela" display="https://fi.wikipedia.org/wiki/Kaarela" xr:uid="{5E1DB4A2-C002-47BF-A9C7-1D95419AD600}"/>
+    <hyperlink ref="C37" r:id="rId29" tooltip="Pakila" display="https://fi.wikipedia.org/wiki/Pakila" xr:uid="{AD3A54AE-E065-401D-AA9D-A7C8E2B1D3EC}"/>
+    <hyperlink ref="C38" r:id="rId30" tooltip="Tuomarinkylä" display="https://fi.wikipedia.org/wiki/Tuomarinkyl%C3%A4" xr:uid="{7BD25363-B127-4D0E-9A04-CD50962E6138}"/>
+    <hyperlink ref="C39" r:id="rId31" tooltip="Viikki" display="https://fi.wikipedia.org/wiki/Viikki" xr:uid="{0DD44024-38FF-428A-9EBD-2292F5DA2875}"/>
+    <hyperlink ref="C40" r:id="rId32" tooltip="Pukinmäki" display="https://fi.wikipedia.org/wiki/Pukinm%C3%A4ki" xr:uid="{FD28F3FC-7C50-4419-BEDE-9471C48D8FB7}"/>
+    <hyperlink ref="C41" r:id="rId33" tooltip="Malmi (Helsinki)" display="https://fi.wikipedia.org/wiki/Malmi_(Helsinki)" xr:uid="{4A68C459-2531-430E-816A-E12539EA34CC}"/>
+    <hyperlink ref="C42" r:id="rId34" tooltip="Tapaninkylä" display="https://fi.wikipedia.org/wiki/Tapaninkyl%C3%A4" xr:uid="{485B25D4-700B-49EF-AA06-8C9106FACBF2}"/>
+    <hyperlink ref="C43" r:id="rId35" tooltip="Suutarila" display="https://fi.wikipedia.org/wiki/Suutarila" xr:uid="{F3BEF9E3-AEF2-47B0-989B-D046CB824D29}"/>
+    <hyperlink ref="C44" r:id="rId36" tooltip="Suurmetsä" display="https://fi.wikipedia.org/wiki/Suurmets%C3%A4" xr:uid="{738A2A16-14A8-4E38-A1B2-FA667BD7849C}"/>
+    <hyperlink ref="C45" r:id="rId37" tooltip="Kulosaari" display="https://fi.wikipedia.org/wiki/Kulosaari" xr:uid="{6626F5D3-9CDE-4F6C-BE42-16EE0ED34E29}"/>
+    <hyperlink ref="C46" r:id="rId38" tooltip="Herttoniemi" display="https://fi.wikipedia.org/wiki/Herttoniemi" xr:uid="{1FE6B6A0-7332-4508-9945-00BF41CB0B60}"/>
+    <hyperlink ref="C47" r:id="rId39" tooltip="Tammisalo" display="https://fi.wikipedia.org/wiki/Tammisalo" xr:uid="{37C9D2BA-3EB0-4B48-9DD0-678505B52616}"/>
+    <hyperlink ref="C48" r:id="rId40" tooltip="Vartiokylä" display="https://fi.wikipedia.org/wiki/Vartiokyl%C3%A4" xr:uid="{18DFC04F-F287-4538-A3E1-624437E9A1DA}"/>
+    <hyperlink ref="C49" r:id="rId41" tooltip="Pitäjänmäki" display="https://fi.wikipedia.org/wiki/Pit%C3%A4j%C3%A4nm%C3%A4ki" xr:uid="{ABBBB111-A233-46EE-8E37-A77A5C7549B2}"/>
+    <hyperlink ref="C50" r:id="rId42" tooltip="Mellunkylä" display="https://fi.wikipedia.org/wiki/Mellunkyl%C3%A4" xr:uid="{CF7909F8-EA7B-48A6-A74F-DDC103A02227}"/>
+    <hyperlink ref="C51" r:id="rId43" tooltip="Vartiosaari" display="https://fi.wikipedia.org/wiki/Vartiosaari" xr:uid="{549A6024-CB6B-429C-B0E9-B3551CC5BB54}"/>
+    <hyperlink ref="C52" r:id="rId44" tooltip="Laajasalo" display="https://fi.wikipedia.org/wiki/Laajasalo" xr:uid="{7AFDF2D1-1E60-4BB5-9546-0CFB2EB8794D}"/>
+    <hyperlink ref="C53" r:id="rId45" tooltip="Villinki" display="https://fi.wikipedia.org/wiki/Villinki" xr:uid="{47516BE1-B62A-45FB-9320-60EF7F53CAAD}"/>
+    <hyperlink ref="C54" r:id="rId46" tooltip="Santahamina" display="https://fi.wikipedia.org/wiki/Santahamina" xr:uid="{12BD6452-F48B-4C64-B336-8FEC6AB3BD69}"/>
+    <hyperlink ref="C55" r:id="rId47" tooltip="Suomenlinna (kaupunginosa)" display="https://fi.wikipedia.org/wiki/Suomenlinna_(kaupunginosa)" xr:uid="{C64A0135-F772-478D-A614-A93F997DA711}"/>
+    <hyperlink ref="C56" r:id="rId48" tooltip="Ulkosaaret" display="https://fi.wikipedia.org/wiki/Ulkosaaret" xr:uid="{670A0707-552B-4471-9E15-547A618273AB}"/>
+    <hyperlink ref="C57" r:id="rId49" tooltip="Vuosaari" display="https://fi.wikipedia.org/wiki/Vuosaari" xr:uid="{5BA36901-4DEA-484A-AE04-E593C448CC86}"/>
+    <hyperlink ref="C58" r:id="rId50" tooltip="Östersundom" display="https://fi.wikipedia.org/wiki/%C3%96stersundom" xr:uid="{D71BE9B7-0C94-48FA-BCE7-872DF1A16FF5}"/>
+    <hyperlink ref="C59" r:id="rId51" tooltip="Salmenkallio" display="https://fi.wikipedia.org/wiki/Salmenkallio" xr:uid="{8AF54BBE-D0A0-46CA-807D-77DC44A47591}"/>
+    <hyperlink ref="C60" r:id="rId52" tooltip="Talosaari" display="https://fi.wikipedia.org/wiki/Talosaari" xr:uid="{261892A3-E4FB-4392-8AFA-941322F900A3}"/>
+    <hyperlink ref="C61" r:id="rId53" tooltip="Karhusaari (Helsinki)" display="https://fi.wikipedia.org/wiki/Karhusaari_(Helsinki)" xr:uid="{D0F9D7F4-E436-41E3-8152-227A8813ADE7}"/>
+    <hyperlink ref="C62" r:id="rId54" tooltip="Ultuna" display="https://fi.wikipedia.org/wiki/Ultuna" xr:uid="{2BF066E9-14B3-4374-88AA-619281AED7F7}"/>
+    <hyperlink ref="C63" r:id="rId55" tooltip="Aluemeri (Helsinki)" display="https://fi.wikipedia.org/wiki/Aluemeri_(Helsinki)" xr:uid="{E80F4FCE-067D-47E6-BF18-84CD4A7871F7}"/>
+    <hyperlink ref="B9" r:id="rId56" tooltip="Eira" display="https://fi.wikipedia.org/wiki/Eira" xr:uid="{453981F0-C686-41BC-BDB1-A2A707CFC582}"/>
+    <hyperlink ref="B10" r:id="rId57" tooltip="Ullanlinna" display="https://fi.wikipedia.org/wiki/Ullanlinna" xr:uid="{17A14A4F-1F23-40C6-ACB9-CE8E3B1D0FCB}"/>
+    <hyperlink ref="B11" r:id="rId58" tooltip="Katajanokka" display="https://fi.wikipedia.org/wiki/Katajanokka" xr:uid="{8A51BEEA-45BD-43AE-AFF2-9D580923F6F4}"/>
+    <hyperlink ref="B12" r:id="rId59" tooltip="Kaivopuisto" display="https://fi.wikipedia.org/wiki/Kaivopuisto" xr:uid="{9B62D7F2-EBB1-4B06-AB13-6E3A2C587825}"/>
+    <hyperlink ref="B13" r:id="rId60" tooltip="Sörnäinen" display="https://fi.wikipedia.org/wiki/S%C3%B6rn%C3%A4inen" xr:uid="{C17C1975-12CC-4A69-8FD9-01D17E90E1DF}"/>
+    <hyperlink ref="B14" r:id="rId61" tooltip="Kallio (Helsinki)" display="https://fi.wikipedia.org/wiki/Kallio_(Helsinki)" xr:uid="{E75795F5-6749-48B4-8C97-A9853968158C}"/>
+    <hyperlink ref="B15" r:id="rId62" tooltip="Alppiharju" display="https://fi.wikipedia.org/wiki/Alppiharju" xr:uid="{B94B3967-8366-449B-864F-3FC9D6F52C18}"/>
+    <hyperlink ref="B16" r:id="rId63" tooltip="Etu-Töölö" display="https://fi.wikipedia.org/wiki/Etu-T%C3%B6%C3%B6l%C3%B6" xr:uid="{E4E139CC-0033-4E86-B48D-D5EDAEB2A6FA}"/>
+    <hyperlink ref="B17" r:id="rId64" tooltip="Taka-Töölö" display="https://fi.wikipedia.org/wiki/Taka-T%C3%B6%C3%B6l%C3%B6" xr:uid="{D5662D37-A729-40C2-ACEE-A183F0A2411A}"/>
+    <hyperlink ref="B18" r:id="rId65" tooltip="Meilahti" display="https://fi.wikipedia.org/wiki/Meilahti" xr:uid="{E9B06415-0AD5-4D38-A510-2EB0E7F3A23C}"/>
+    <hyperlink ref="B19" r:id="rId66" tooltip="Ruskeasuo" display="https://fi.wikipedia.org/wiki/Ruskeasuo" xr:uid="{26172DED-3C57-49D1-B3A4-947846122B7C}"/>
+    <hyperlink ref="B20" r:id="rId67" tooltip="Pasila" display="https://fi.wikipedia.org/wiki/Pasila" xr:uid="{74084596-71D8-4A2A-B0D8-1A6DE42A0AB3}"/>
+    <hyperlink ref="B21" r:id="rId68" tooltip="Laakso (Helsinki)" display="https://fi.wikipedia.org/wiki/Laakso_(Helsinki)" xr:uid="{311FB38D-BC01-4539-B3F4-8091A00CCEBB}"/>
+    <hyperlink ref="B22" r:id="rId69" tooltip="Mustikkamaa-Korkeasaari" display="https://fi.wikipedia.org/wiki/Mustikkamaa-Korkeasaari" xr:uid="{860B1357-AB24-463D-85DE-5049E91EA62B}"/>
+    <hyperlink ref="B23" r:id="rId70" tooltip="Länsisatama (Helsinki)" display="https://fi.wikipedia.org/wiki/L%C3%A4nsisatama_(Helsinki)" xr:uid="{668F16A6-BE4C-43DF-80D3-13253A40A752}"/>
+    <hyperlink ref="B24" r:id="rId71" tooltip="Hermanni (Helsinki)" display="https://fi.wikipedia.org/wiki/Hermanni_(Helsinki)" xr:uid="{576A40B6-D1E4-4024-A1CC-E22D9D429DFF}"/>
+    <hyperlink ref="B25" r:id="rId72" tooltip="Vallila" display="https://fi.wikipedia.org/wiki/Vallila" xr:uid="{64B904EF-74D0-4916-9640-290C829384FA}"/>
+    <hyperlink ref="B26" r:id="rId73" tooltip="Toukola" display="https://fi.wikipedia.org/wiki/Toukola" xr:uid="{2599A8DE-0D2D-40C3-BC48-33D6E2F53D12}"/>
+    <hyperlink ref="B27" r:id="rId74" tooltip="Kumpula" display="https://fi.wikipedia.org/wiki/Kumpula" xr:uid="{78026101-0E82-4ADC-BCA6-250C05538753}"/>
+    <hyperlink ref="B28" r:id="rId75" tooltip="Käpylä" display="https://fi.wikipedia.org/wiki/K%C3%A4pyl%C3%A4" xr:uid="{E04BD58E-F34A-4B8B-BFFA-0FCF2D5C2C5F}"/>
+    <hyperlink ref="B29" r:id="rId76" tooltip="Koskela (Helsinki)" display="https://fi.wikipedia.org/wiki/Koskela_(Helsinki)" xr:uid="{394DA44F-9C70-43B5-83B7-966347E354B3}"/>
+    <hyperlink ref="B30" r:id="rId77" tooltip="Vanhakaupunki (Helsinki)" display="https://fi.wikipedia.org/wiki/Vanhakaupunki_(Helsinki)" xr:uid="{03B4F839-5572-4802-9D4C-FA62A4961B06}"/>
+    <hyperlink ref="B31" r:id="rId78" tooltip="Oulunkylä" display="https://fi.wikipedia.org/wiki/Oulunkyl%C3%A4" xr:uid="{4759A816-6928-40DB-95A0-DE8BABC7D668}"/>
+    <hyperlink ref="B32" r:id="rId79" tooltip="Haaga" display="https://fi.wikipedia.org/wiki/Haaga" xr:uid="{15986C9A-9BD5-43C0-AC45-897EBEB131B0}"/>
+    <hyperlink ref="B33" r:id="rId80" tooltip="Munkkiniemi" display="https://fi.wikipedia.org/wiki/Munkkiniemi" xr:uid="{E8434F1C-0D82-48F7-BBAF-B79EE2B1EE69}"/>
+    <hyperlink ref="B34" r:id="rId81" tooltip="Lauttasaari" display="https://fi.wikipedia.org/wiki/Lauttasaari" xr:uid="{9317EF73-FEE6-4C68-BDE1-DE447C6D6145}"/>
+    <hyperlink ref="B35" r:id="rId82" tooltip="Konala" display="https://fi.wikipedia.org/wiki/Konala" xr:uid="{A4540894-A1A0-4DD7-B8B3-BE2CDDA2DC26}"/>
+    <hyperlink ref="B36" r:id="rId83" tooltip="Kaarela" display="https://fi.wikipedia.org/wiki/Kaarela" xr:uid="{3914718C-5412-49F3-B2B5-B7DA94990BF3}"/>
+    <hyperlink ref="B37" r:id="rId84" tooltip="Pakila" display="https://fi.wikipedia.org/wiki/Pakila" xr:uid="{9116858B-FD8F-46B2-9F98-3461965CD1F9}"/>
+    <hyperlink ref="B38" r:id="rId85" tooltip="Tuomarinkylä" display="https://fi.wikipedia.org/wiki/Tuomarinkyl%C3%A4" xr:uid="{7171BA34-8B16-4F9B-91B5-B30FD6A31D8C}"/>
+    <hyperlink ref="B39" r:id="rId86" tooltip="Viikki" display="https://fi.wikipedia.org/wiki/Viikki" xr:uid="{3A14DA02-EEA3-44F1-872C-7753C7692F39}"/>
+    <hyperlink ref="B40" r:id="rId87" tooltip="Pukinmäki" display="https://fi.wikipedia.org/wiki/Pukinm%C3%A4ki" xr:uid="{8BC9B1A4-9CFC-4275-962C-871AF5343862}"/>
+    <hyperlink ref="B41" r:id="rId88" tooltip="Malmi (Helsinki)" display="https://fi.wikipedia.org/wiki/Malmi_(Helsinki)" xr:uid="{CF9903CF-A41E-4F48-9BA4-032D9F4560B7}"/>
+    <hyperlink ref="B42" r:id="rId89" tooltip="Tapaninkylä" display="https://fi.wikipedia.org/wiki/Tapaninkyl%C3%A4" xr:uid="{B10CAD78-B2DD-4C6D-ACED-B4A7847B5B5A}"/>
+    <hyperlink ref="B43" r:id="rId90" tooltip="Suutarila" display="https://fi.wikipedia.org/wiki/Suutarila" xr:uid="{C79CE8F0-E8BC-48A0-B4D2-F5C5B762CCC6}"/>
+    <hyperlink ref="B44" r:id="rId91" tooltip="Suurmetsä" display="https://fi.wikipedia.org/wiki/Suurmets%C3%A4" xr:uid="{6F259981-11C9-4EC3-8B17-0EDB4A186B1A}"/>
+    <hyperlink ref="B45" r:id="rId92" tooltip="Kulosaari" display="https://fi.wikipedia.org/wiki/Kulosaari" xr:uid="{16D1427B-9EFF-45F6-81A3-2EC57C0FE569}"/>
+    <hyperlink ref="B46" r:id="rId93" tooltip="Herttoniemi" display="https://fi.wikipedia.org/wiki/Herttoniemi" xr:uid="{BCF3BDF5-F822-4DE3-8C57-9B7025567065}"/>
+    <hyperlink ref="B47" r:id="rId94" tooltip="Tammisalo" display="https://fi.wikipedia.org/wiki/Tammisalo" xr:uid="{66D232B6-E8F5-4A27-B58C-9A92C667AB00}"/>
+    <hyperlink ref="B48" r:id="rId95" tooltip="Vartiokylä" display="https://fi.wikipedia.org/wiki/Vartiokyl%C3%A4" xr:uid="{0B5849BA-F320-43DE-9855-3988B1A1DC63}"/>
+    <hyperlink ref="B49" r:id="rId96" tooltip="Pitäjänmäki" display="https://fi.wikipedia.org/wiki/Pit%C3%A4j%C3%A4nm%C3%A4ki" xr:uid="{D77069C1-2474-41DA-AC28-945B02FE9AD6}"/>
+    <hyperlink ref="B50" r:id="rId97" tooltip="Mellunkylä" display="https://fi.wikipedia.org/wiki/Mellunkyl%C3%A4" xr:uid="{1CB56DA8-54D0-4DD6-8745-E3C513725069}"/>
+    <hyperlink ref="B51" r:id="rId98" tooltip="Vartiosaari" display="https://fi.wikipedia.org/wiki/Vartiosaari" xr:uid="{BD307EF1-5336-4A18-A7EA-BE2DA531BB53}"/>
+    <hyperlink ref="B52" r:id="rId99" tooltip="Laajasalo" display="https://fi.wikipedia.org/wiki/Laajasalo" xr:uid="{E418DFD1-0347-47C3-ABA8-E2855627A587}"/>
+    <hyperlink ref="B53" r:id="rId100" tooltip="Villinki" display="https://fi.wikipedia.org/wiki/Villinki" xr:uid="{F54122D3-44F5-40E7-B41D-FA9A7172BA32}"/>
+    <hyperlink ref="B54" r:id="rId101" tooltip="Santahamina" display="https://fi.wikipedia.org/wiki/Santahamina" xr:uid="{CDB6334A-5ED6-474E-B327-32F69EF818E9}"/>
+    <hyperlink ref="B55" r:id="rId102" tooltip="Suomenlinna (kaupunginosa)" display="https://fi.wikipedia.org/wiki/Suomenlinna_(kaupunginosa)" xr:uid="{A59193F1-F431-4A59-B808-AF0BADD09F07}"/>
+    <hyperlink ref="B56" r:id="rId103" tooltip="Ulkosaaret" display="https://fi.wikipedia.org/wiki/Ulkosaaret" xr:uid="{52B172B6-11C5-48BE-9436-03B095FE324F}"/>
+    <hyperlink ref="B57" r:id="rId104" tooltip="Vuosaari" display="https://fi.wikipedia.org/wiki/Vuosaari" xr:uid="{D83DA05D-FBFF-48BB-ABDC-47BD776D3418}"/>
+    <hyperlink ref="B58" r:id="rId105" tooltip="Östersundom" display="https://fi.wikipedia.org/wiki/%C3%96stersundom" xr:uid="{09EA3BB2-23A0-4B84-B7A2-1D59479B3457}"/>
+    <hyperlink ref="B59" r:id="rId106" tooltip="Salmenkallio" display="https://fi.wikipedia.org/wiki/Salmenkallio" xr:uid="{08E20A28-B1A2-4773-918D-544FCE1D1D37}"/>
+    <hyperlink ref="B60" r:id="rId107" tooltip="Talosaari" display="https://fi.wikipedia.org/wiki/Talosaari" xr:uid="{64068612-B018-45CF-9775-95225327517C}"/>
+    <hyperlink ref="B61" r:id="rId108" tooltip="Karhusaari (Helsinki)" display="https://fi.wikipedia.org/wiki/Karhusaari_(Helsinki)" xr:uid="{FE4F9380-893C-40EC-AB94-2A0EDB87A776}"/>
+    <hyperlink ref="B62" r:id="rId109" tooltip="Ultuna" display="https://fi.wikipedia.org/wiki/Ultuna" xr:uid="{9A50E321-8A86-46B2-BB1C-5B965F0C8CA0}"/>
+    <hyperlink ref="B63" r:id="rId110" tooltip="Aluemeri (Helsinki)" display="https://fi.wikipedia.org/wiki/Aluemeri_(Helsinki)" xr:uid="{A2CF1590-FD86-4D54-836D-F2B6C49F3F69}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1727,7 +3479,7 @@
         <v>75</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C2" s="4"/>
     </row>
@@ -1749,7 +3501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{549C78AA-1218-455B-9887-3E0A5E59C6C7}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6:B8"/>
     </sheetView>
   </sheetViews>
@@ -1803,40 +3555,40 @@
         <v>74</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>151</v>
+        <v>131</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>152</v>
+        <v>132</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>153</v>
+        <v>133</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>95</v>
@@ -1845,7 +3597,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>96</v>
@@ -1854,10 +3606,10 @@
     </row>
     <row r="11" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C11" s="4"/>
     </row>
@@ -1872,7 +3624,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B3"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1898,8 +3650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A280385-38F0-446C-9432-C0DF8BDF752B}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1921,10 +3673,10 @@
         <v>58</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>63</v>
@@ -1940,8 +3692,8 @@
       <c r="C2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>60</v>
+      <c r="D2" s="25" t="s">
+        <v>341</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>60</v>
@@ -1958,8 +3710,8 @@
       <c r="C3" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>65</v>
+      <c r="D3" s="25" t="s">
+        <v>342</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>65</v>
@@ -1977,8 +3729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF16B1B1-A6B4-4B56-9813-CCF1B731EDAC}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D6"/>
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2024,10 +3776,10 @@
         <v>45</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>35</v>
@@ -2051,10 +3803,10 @@
         <v>42</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="S1" s="3" t="s">
         <v>11</v>
@@ -2073,8 +3825,8 @@
       <c r="C2" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="27" t="s">
-        <v>154</v>
+      <c r="D2" s="6" t="s">
+        <v>149</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>77</v>
@@ -2135,8 +3887,8 @@
       <c r="C3" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="27" t="s">
-        <v>155</v>
+      <c r="D3" s="6" t="s">
+        <v>150</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>49</v>
@@ -2197,8 +3949,8 @@
       <c r="C4" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="27" t="s">
-        <v>156</v>
+      <c r="D4" s="6" t="s">
+        <v>151</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>50</v>
@@ -2259,8 +4011,8 @@
       <c r="C5" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="27" t="s">
-        <v>157</v>
+      <c r="D5" s="6" t="s">
+        <v>152</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>51</v>
@@ -2271,8 +4023,8 @@
       <c r="G5" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>114</v>
+      <c r="H5" s="26" t="s">
+        <v>343</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>114</v>
@@ -2321,8 +4073,8 @@
       <c r="C6" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="D6" s="28" t="s">
-        <v>158</v>
+      <c r="D6" s="19" t="s">
+        <v>153</v>
       </c>
       <c r="E6" s="19" t="s">
         <v>112</v>
@@ -2333,8 +4085,8 @@
       <c r="G6" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="H6" s="21" t="s">
-        <v>115</v>
+      <c r="H6" s="27" t="s">
+        <v>344</v>
       </c>
       <c r="I6" s="21" t="s">
         <v>115</v>
@@ -2343,10 +4095,10 @@
         <v>72</v>
       </c>
       <c r="K6" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="L6" s="23" t="s">
-        <v>131</v>
+        <v>128</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>161</v>
       </c>
       <c r="M6" s="20" t="s">
         <v>93</v>
@@ -2355,7 +4107,7 @@
         <v>67</v>
       </c>
       <c r="O6" s="24" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="P6" s="22" t="s">
         <v>72</v>
@@ -2377,8 +4129,8 @@
   <hyperlinks>
     <hyperlink ref="L5" r:id="rId1" display="johndoe@outlook" xr:uid="{343BA063-0012-4384-B796-30762B791B20}"/>
     <hyperlink ref="I6" r:id="rId2" display="https://www.insee.fr/fr/metadonnees/geographie/departement/78-yvelines" xr:uid="{E9DB7908-5FDA-4050-8A5F-E04BE4CA97B2}"/>
-    <hyperlink ref="H6" r:id="rId3" display="https://www.insee.fr/fr/metadonnees/geographie/departement/78-yvelines" xr:uid="{0CC2A5A6-44DC-4BA9-90B5-BBDDD2C1FD09}"/>
-    <hyperlink ref="G6" r:id="rId4" display="https://www.insee.fr/fr/metadonnees/geographie/departement/78-yvelines" xr:uid="{35EF75D7-E3B5-4B3D-90F0-676958195AB2}"/>
+    <hyperlink ref="G6" r:id="rId3" display="https://www.insee.fr/fr/metadonnees/geographie/departement/78-yvelines" xr:uid="{35EF75D7-E3B5-4B3D-90F0-676958195AB2}"/>
+    <hyperlink ref="H6" r:id="rId4" location="tonttipalvelujen-yhteystiedot-kartalla" xr:uid="{0CC2A5A6-44DC-4BA9-90B5-BBDDD2C1FD09}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
@@ -2438,18 +4190,18 @@
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>82</v>
+        <v>144</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>345</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>82</v>

</xml_diff>

<commit_message>
Update for next version of AISA
</commit_message>
<xml_diff>
--- a/runtime/apps/AISA/AISA.xlsx
+++ b/runtime/apps/AISA/AISA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\athena\github\trusted-service\runtime\apps\AISA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4829A5-1448-4B4C-BFAA-F2F2C6FA1E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396F3034-5407-4716-93CF-0ABF593C4A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-360" yWindow="0" windowWidth="15465" windowHeight="15480" tabRatio="973" firstSheet="7" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="973" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="APP &amp; MODEL" sheetId="25" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="364">
   <si>
     <t>Parameter</t>
   </si>
@@ -440,9 +440,6 @@
   </si>
   <si>
     <t>districts</t>
-  </si>
-  <si>
-    <t>city_plots_for_sports_and_sporting_activities commercial_plots</t>
   </si>
   <si>
     <t>Dear city of Helsinki building services,
@@ -504,14 +501,6 @@
     <t>Tämä sovellus on tarkoitettu kaupungin tontti- ja rakennuslupa-asioihin</t>
   </si>
   <si>
-    <t>Hei,
-tarvitsisin tonttia seuraaviin käyttötarkoituksiin:
-- uuden kuntosalin rakentamiseen
-- ravintolan rakentamiseen
-- kerrostaloasuinrakentamiseen
-Osaatteko auttaa?</t>
-  </si>
-  <si>
     <t>Päivämäärä</t>
   </si>
   <si>
@@ -1100,8 +1089,70 @@
     <t>https://www.hel.fi/fi/kaupunkiymparisto-ja-liikenne/tontit-ja-rakentamisen-luvat/yhteystiedot-rakennusvalvonta-tontit-ja-lupa-asiat#tonttipalvelujen-yhteystiedot-kartalla</t>
   </si>
   <si>
-    <t>Tänään on {date_message} (DD/MM/YYYY).  
+    <t>Rule</t>
+  </si>
+  <si>
+    <t>email to …</t>
+  </si>
+  <si>
+    <t>goto page</t>
+  </si>
+  <si>
+    <t>Additional question</t>
+  </si>
+  <si>
+    <t>What sports?</t>
+  </si>
+  <si>
+    <t>If sport == "table tennis" then send email to table_tennis_plots@helsinki.fi else goto web site sports@helsinki.fi</t>
+  </si>
+  <si>
+    <t>District(s) (list or link), 
+Planning timeframe -less than a year, about year, over a year
+Related issues</t>
+  </si>
+  <si>
+    <t>planning_date</t>
+  </si>
+  <si>
+    <t>When do you want to start?</t>
+  </si>
+  <si>
+    <t>Date of start of works formatted as DD/MM/YYYY</t>
+  </si>
+  <si>
+    <t>EXTRACT AND HIGHLIGHT</t>
+  </si>
+  <si>
+    <t>city plots for apartment blocks and terraced houses</t>
+  </si>
+  <si>
+    <t>Tänään on {date_message} (PP/KK/VVVV).  
 Olet asiakaspalvelija, joka arvioi ja ohjaa kyselyjä eteenpäin asiakaspalvelutiimeille.</t>
+  </si>
+  <si>
+    <t>Milloin haluat aloittaa?</t>
+  </si>
+  <si>
+    <t>Työn suunniteltu aloitus formaatissa PP/KK/VVVV</t>
+  </si>
+  <si>
+    <t>Mikä on rakennustyön suunniteltu aloituspäivä?</t>
+  </si>
+  <si>
+    <t>I want to rent a plot for building apartments in a year and a half, ot so. Please let me know how to proceed.</t>
+  </si>
+  <si>
+    <t>Haluaisin vuokrata tontin kerrostaloasuntojen rakentamista varten noin puolentoista vuoden kuluttua. Miten minun tulisi edetä?</t>
+  </si>
+  <si>
+    <t>Other example</t>
+  </si>
+  <si>
+    <t>Suunnittelen ostoskeskuksen rakentamista. Onko kaupungilla sopivia tontteja?</t>
+  </si>
+  <si>
+    <t>I want to construct a shopping center. Is there a plot available for that?</t>
   </si>
 </sst>
 </file>
@@ -1151,7 +1202,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1178,6 +1229,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1211,7 +1268,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1260,8 +1317,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="2" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1562,235 +1632,274 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40884519-E9E2-4702-AA20-B46B229B9942}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="86" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="61.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="56" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="103.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="61.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="28" t="s">
+        <v>346</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>343</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="G5" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>154</v>
-      </c>
       <c r="F6" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="I6" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>155</v>
-      </c>
       <c r="F7" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="I7" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>156</v>
-      </c>
       <c r="F8" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="I8" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>157</v>
-      </c>
       <c r="F9" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="I9" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>158</v>
-      </c>
       <c r="F10" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="I10" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>159</v>
-      </c>
       <c r="F11" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="I11" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>160</v>
-      </c>
       <c r="F12" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="I12" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13"/>
-      <c r="B13"/>
-      <c r="C13"/>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13"/>
-      <c r="G13"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14"/>
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14"/>
-      <c r="G14"/>
+    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="F13" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="G13" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>354</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1897,7 +2006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD020DE-44B7-44EF-BEA3-8491F2595E0A}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
@@ -2038,7 +2147,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="W28" sqref="W28"/>
+      <selection activeCell="Y28" sqref="Y28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2051,7 +2160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48C25835-C93B-43AA-B5BF-FF69903103A9}">
   <dimension ref="A1:R63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -2097,16 +2206,16 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>161</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>163</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>67</v>
@@ -2124,16 +2233,16 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>164</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>166</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>67</v>
@@ -2151,16 +2260,16 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>167</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>169</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>67</v>
@@ -2178,16 +2287,16 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>170</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>172</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>67</v>
@@ -2205,16 +2314,16 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>173</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>175</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>67</v>
@@ -2232,16 +2341,16 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>176</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>178</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>67</v>
@@ -2252,16 +2361,16 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>179</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>181</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>67</v>
@@ -2272,16 +2381,16 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>182</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>184</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>67</v>
@@ -2292,16 +2401,16 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>185</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>187</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>67</v>
@@ -2312,16 +2421,16 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>67</v>
@@ -2332,16 +2441,16 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>193</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>67</v>
@@ -2352,16 +2461,16 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>196</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>67</v>
@@ -2372,16 +2481,16 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>197</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>199</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>67</v>
@@ -2392,16 +2501,16 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>200</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>202</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>67</v>
@@ -2412,16 +2521,16 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>203</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>205</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>67</v>
@@ -2432,16 +2541,16 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>206</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>208</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>67</v>
@@ -2452,16 +2561,16 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>209</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>211</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>67</v>
@@ -2472,16 +2581,16 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>212</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>214</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>67</v>
@@ -2492,16 +2601,16 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>215</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>217</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>67</v>
@@ -2512,16 +2621,16 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>218</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>220</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>67</v>
@@ -2532,16 +2641,16 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>221</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>223</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>67</v>
@@ -2552,16 +2661,16 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>224</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>226</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>67</v>
@@ -2572,16 +2681,16 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>227</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>229</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>67</v>
@@ -2592,16 +2701,16 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>230</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>232</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>67</v>
@@ -2612,16 +2721,16 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>233</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>235</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>67</v>
@@ -2632,16 +2741,16 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="D29" s="6" t="s">
         <v>236</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>238</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>67</v>
@@ -2652,16 +2761,16 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="D30" s="6" t="s">
         <v>239</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>241</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>67</v>
@@ -2672,16 +2781,16 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="D31" s="6" t="s">
         <v>242</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>244</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>67</v>
@@ -2693,16 +2802,16 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="D32" s="6" t="s">
         <v>245</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>247</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>67</v>
@@ -2713,16 +2822,16 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="D33" s="6" t="s">
         <v>248</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>250</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>67</v>
@@ -2733,16 +2842,16 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="D34" s="6" t="s">
         <v>251</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>253</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>67</v>
@@ -2753,16 +2862,16 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="D35" s="6" t="s">
         <v>254</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>256</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>67</v>
@@ -2773,16 +2882,16 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="D36" s="6" t="s">
         <v>257</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>258</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>258</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>259</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>67</v>
@@ -2793,16 +2902,16 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="D37" s="6" t="s">
         <v>260</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>262</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>67</v>
@@ -2813,16 +2922,16 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="D38" s="6" t="s">
         <v>263</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>265</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>67</v>
@@ -2833,16 +2942,16 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="D39" s="6" t="s">
         <v>266</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>268</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>67</v>
@@ -2853,16 +2962,16 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="D40" s="6" t="s">
         <v>269</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>271</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>67</v>
@@ -2873,16 +2982,16 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="D41" s="6" t="s">
         <v>272</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>274</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>67</v>
@@ -2893,16 +3002,16 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="D42" s="6" t="s">
         <v>275</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>277</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>67</v>
@@ -2913,16 +3022,16 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="D43" s="6" t="s">
         <v>278</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>280</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>67</v>
@@ -2933,16 +3042,16 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="D44" s="6" t="s">
         <v>281</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>283</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>67</v>
@@ -2953,16 +3062,16 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="D45" s="6" t="s">
         <v>284</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>286</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>67</v>
@@ -2973,16 +3082,16 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="D46" s="6" t="s">
         <v>287</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>289</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>67</v>
@@ -2993,16 +3102,16 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="D47" s="6" t="s">
         <v>290</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>292</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>67</v>
@@ -3013,16 +3122,16 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="D48" s="6" t="s">
         <v>293</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>294</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>294</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>295</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>67</v>
@@ -3033,16 +3142,16 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="D49" s="6" t="s">
         <v>296</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>297</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>297</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>298</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>67</v>
@@ -3053,16 +3162,16 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="D50" s="6" t="s">
         <v>299</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>301</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>67</v>
@@ -3073,16 +3182,16 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="D51" s="6" t="s">
         <v>302</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>303</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>303</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>304</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>67</v>
@@ -3093,16 +3202,16 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="D52" s="6" t="s">
         <v>305</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>306</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>306</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>307</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>67</v>
@@ -3113,16 +3222,16 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="D53" s="6" t="s">
         <v>308</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>309</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>309</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>310</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>67</v>
@@ -3133,16 +3242,16 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="D54" s="6" t="s">
         <v>311</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>313</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>67</v>
@@ -3153,16 +3262,16 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="D55" s="6" t="s">
         <v>314</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="C55" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="D55" s="6" t="s">
-        <v>316</v>
       </c>
       <c r="E55" s="6" t="s">
         <v>67</v>
@@ -3173,16 +3282,16 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="D56" s="6" t="s">
         <v>317</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>319</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>67</v>
@@ -3193,16 +3302,16 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="D57" s="6" t="s">
         <v>320</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>321</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>321</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>322</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>67</v>
@@ -3213,16 +3322,16 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="D58" s="6" t="s">
         <v>323</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>324</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>324</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>325</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>67</v>
@@ -3233,16 +3342,16 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="D59" s="6" t="s">
         <v>326</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>327</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>327</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>328</v>
       </c>
       <c r="E59" s="6" t="s">
         <v>67</v>
@@ -3253,16 +3362,16 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="D60" s="6" t="s">
         <v>329</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>330</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>330</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>331</v>
       </c>
       <c r="E60" s="6" t="s">
         <v>67</v>
@@ -3273,16 +3382,16 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="D61" s="6" t="s">
         <v>332</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>333</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>333</v>
-      </c>
-      <c r="D61" s="6" t="s">
-        <v>334</v>
       </c>
       <c r="E61" s="6" t="s">
         <v>67</v>
@@ -3293,16 +3402,16 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="D62" s="6" t="s">
         <v>335</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>336</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>336</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>337</v>
       </c>
       <c r="E62" s="6" t="s">
         <v>67</v>
@@ -3313,16 +3422,16 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="D63" s="6" t="s">
         <v>338</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>339</v>
-      </c>
-      <c r="C63" s="6" t="s">
-        <v>339</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>340</v>
       </c>
       <c r="E63" s="6" t="s">
         <v>67</v>
@@ -3479,7 +3588,7 @@
         <v>75</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C2" s="4"/>
     </row>
@@ -3499,10 +3608,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{549C78AA-1218-455B-9887-3E0A5E59C6C7}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B8"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3550,45 +3659,45 @@
       </c>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>130</v>
+        <v>359</v>
       </c>
       <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>148</v>
+      <c r="B8" t="s">
+        <v>360</v>
       </c>
       <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>95</v>
@@ -3597,7 +3706,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>96</v>
@@ -3606,12 +3715,27 @@
     </row>
     <row r="11" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C11" s="4"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="33" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>363</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3651,7 +3775,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D3"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3673,10 +3797,10 @@
         <v>58</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>141</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>63</v>
@@ -3693,7 +3817,7 @@
         <v>61</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>60</v>
@@ -3711,7 +3835,7 @@
         <v>66</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>65</v>
@@ -3727,10 +3851,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF16B1B1-A6B4-4B56-9813-CCF1B731EDAC}">
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:H6"/>
+    <sheetView topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3776,10 +3900,10 @@
         <v>45</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>142</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>143</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>35</v>
@@ -3803,10 +3927,10 @@
         <v>42</v>
       </c>
       <c r="Q1" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="R1" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>138</v>
       </c>
       <c r="S1" s="3" t="s">
         <v>11</v>
@@ -3826,7 +3950,7 @@
         <v>77</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>77</v>
@@ -3888,7 +4012,7 @@
         <v>49</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>49</v>
@@ -3950,7 +4074,7 @@
         <v>50</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>50</v>
@@ -4012,7 +4136,7 @@
         <v>51</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>51</v>
@@ -4024,7 +4148,7 @@
         <v>114</v>
       </c>
       <c r="H5" s="26" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>114</v>
@@ -4074,7 +4198,7 @@
         <v>112</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E6" s="19" t="s">
         <v>112</v>
@@ -4086,7 +4210,7 @@
         <v>115</v>
       </c>
       <c r="H6" s="27" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="I6" s="21" t="s">
         <v>115</v>
@@ -4098,7 +4222,7 @@
         <v>128</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="M6" s="20" t="s">
         <v>93</v>
@@ -4107,7 +4231,7 @@
         <v>67</v>
       </c>
       <c r="O6" s="24" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="P6" s="22" t="s">
         <v>72</v>
@@ -4122,6 +4246,68 @@
         <v>12</v>
       </c>
       <c r="T6" s="20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>350</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>351</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>356</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>351</v>
+      </c>
+      <c r="F7" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" s="30" t="s">
+        <v>358</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="M7" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="N7" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="O7" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="Q7" s="26" t="s">
+        <v>357</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="S7" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="T7" s="20" t="s">
         <v>67</v>
       </c>
     </row>
@@ -4159,7 +4345,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4192,16 +4378,16 @@
     </row>
     <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>345</v>
+        <v>143</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>355</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>82</v>

</xml_diff>

<commit_message>
Make lint + fix (ruff and eslint) Move email passwords to .env files Start backend only if email passwords in .env file and SMTP connexion ok (lenient mode available), added some other before-start validation Added delphes78audit Made backend available from frontend only Updated documentation Hide console.log in frontend when server is production
</commit_message>
<xml_diff>
--- a/runtime/apps/AISA/AISA.xlsx
+++ b/runtime/apps/AISA/AISA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\athena\github\trusted-service\runtime\apps\AISA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joel/Documents/Dev/Athena/new/trusted-service/runtime/apps/AISA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396F3034-5407-4716-93CF-0ABF593C4A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE7A36E-161B-A94E-B068-371541EF86F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="973" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="29040" windowHeight="15720" tabRatio="973" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="APP &amp; MODEL" sheetId="25" r:id="rId1"/>
@@ -120,12 +120,6 @@
     <t>smtp_server</t>
   </si>
   <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>bceo rdxm suuv orul</t>
-  </si>
-  <si>
     <t>smtp.gmail.com</t>
   </si>
   <si>
@@ -1153,6 +1147,12 @@
   </si>
   <si>
     <t>I want to construct a shopping center. Is there a plot available for that?</t>
+  </si>
+  <si>
+    <t>password_key</t>
+  </si>
+  <si>
+    <t>EMAIL_PASSWORD_ENVOIS_HIBOU</t>
   </si>
 </sst>
 </file>
@@ -1335,9 +1335,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Satisfaisant" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1624,7 +1624,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1634,271 +1634,271 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40884519-E9E2-4702-AA20-B46B229B9942}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="86" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="56" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="103.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="9" width="61.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="103.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="61.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>42</v>
-      </c>
       <c r="F5" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="31" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="F13" s="32" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G13" s="32" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -1918,7 +1918,7 @@
       <selection activeCell="V30" sqref="V30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1932,53 +1932,53 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="64.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.140625" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.1640625" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1996,7 +1996,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2006,18 +2006,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD020DE-44B7-44EF-BEA3-8491F2595E0A}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.5703125" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2028,69 +2028,69 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>30</v>
-      </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>31</v>
-      </c>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>22</v>
+        <v>362</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="B7" s="4">
         <v>587</v>
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2109,23 +2109,23 @@
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="21.7109375" customWidth="1"/>
+    <col min="1" max="2" width="21.6640625" customWidth="1"/>
     <col min="3" max="3" width="101" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
     <col min="5" max="5" width="101" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>18</v>
@@ -2150,7 +2150,7 @@
       <selection activeCell="Y28" sqref="Y28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2164,1280 +2164,1280 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="93.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="93.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.140625" customWidth="1"/>
-    <col min="10" max="10" width="27.28515625" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.1640625" customWidth="1"/>
+    <col min="10" max="10" width="27.33203125" customWidth="1"/>
+    <col min="12" max="12" width="8.83203125" customWidth="1"/>
     <col min="13" max="13" width="26" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.85546875" customWidth="1"/>
+    <col min="16" max="16" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>161</v>
-      </c>
       <c r="E4" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I4" s="17"/>
       <c r="Q4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="R4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>164</v>
-      </c>
       <c r="E5" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I5" s="17"/>
       <c r="Q5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="R5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>167</v>
-      </c>
       <c r="E6" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I6" s="17"/>
       <c r="Q6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="R6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>170</v>
-      </c>
       <c r="E7" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I7" s="17"/>
       <c r="Q7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="R7" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>173</v>
-      </c>
       <c r="E8" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I8" s="17"/>
       <c r="Q8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="R8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="E9" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="D9" s="6" t="s">
+      <c r="B10" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="C10" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="E10" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="D10" s="6" t="s">
+      <c r="B11" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="C11" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="E11" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="D11" s="6" t="s">
+      <c r="B12" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="C12" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="E12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="D12" s="6" t="s">
+      <c r="B13" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="C13" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="E13" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="B14" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="C14" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="E14" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="D14" s="6" t="s">
+      <c r="B15" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="C15" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="E15" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="D15" s="6" t="s">
+      <c r="B16" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="C16" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="E16" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="D16" s="6" t="s">
+      <c r="B17" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="C17" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="E17" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="D17" s="6" t="s">
+      <c r="B18" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="C18" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="E18" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="D18" s="6" t="s">
+      <c r="B19" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="C19" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="E19" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="D19" s="6" t="s">
+      <c r="B20" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="C20" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="E20" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="D20" s="6" t="s">
+      <c r="B21" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="C21" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="E21" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="D21" s="6" t="s">
+      <c r="B22" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="E21" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="C22" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="E22" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="C22" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="D22" s="6" t="s">
+      <c r="B23" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="E22" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="C23" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="E23" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="D23" s="6" t="s">
+      <c r="B24" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="E23" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="C24" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="E24" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="D24" s="6" t="s">
+      <c r="B25" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="E24" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="C25" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="E25" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="D25" s="6" t="s">
+      <c r="B26" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="E25" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="C26" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="E26" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="D26" s="6" t="s">
+      <c r="B27" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="E26" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="C27" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="E27" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="C27" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="D27" s="6" t="s">
+      <c r="B28" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="E27" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="C28" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="E28" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="D28" s="6" t="s">
+      <c r="B29" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="E28" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="C29" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="D29" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="E29" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="D29" s="6" t="s">
+      <c r="B30" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="E29" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="C30" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="D30" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="E30" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="C30" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="D30" s="6" t="s">
+      <c r="B31" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="E30" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="C31" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="D31" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="E31" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="I31" s="16"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="C31" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="D31" s="6" t="s">
+      <c r="B32" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="E31" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="I31" s="16"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+      <c r="C32" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="D32" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="E32" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="C32" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="D32" s="6" t="s">
+      <c r="B33" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="E32" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
+      <c r="C33" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="D33" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="E33" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="C33" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="D33" s="6" t="s">
+      <c r="B34" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="E33" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+      <c r="C34" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="D34" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="E34" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="C34" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="D34" s="6" t="s">
+      <c r="B35" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="E34" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
+      <c r="C35" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="D35" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="E35" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="C35" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="D35" s="6" t="s">
+      <c r="B36" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="E35" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
+      <c r="C36" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="D36" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="E36" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="C36" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="D36" s="6" t="s">
+      <c r="B37" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="E36" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
+      <c r="C37" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="D37" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="E37" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="C37" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="D37" s="6" t="s">
+      <c r="B38" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="E37" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
+      <c r="C38" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="D38" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="E38" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="C38" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="D38" s="6" t="s">
+      <c r="B39" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="E38" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
+      <c r="C39" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="D39" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="E39" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="C39" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="D39" s="6" t="s">
+      <c r="B40" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="E39" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
+      <c r="C40" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="D40" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="E40" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="C40" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="D40" s="6" t="s">
+      <c r="B41" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="E40" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
+      <c r="C41" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="D41" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="E41" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="C41" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="D41" s="6" t="s">
+      <c r="B42" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="E41" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
+      <c r="C42" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="D42" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="E42" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="C42" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="D42" s="6" t="s">
+      <c r="B43" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="E42" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
+      <c r="C43" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="D43" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="E43" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="C43" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="D43" s="6" t="s">
+      <c r="B44" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="E43" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
+      <c r="C44" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="D44" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="E44" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="C44" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="D44" s="6" t="s">
+      <c r="B45" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="E44" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
+      <c r="C45" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="D45" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="E45" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="C45" s="6" t="s">
-        <v>283</v>
-      </c>
-      <c r="D45" s="6" t="s">
+      <c r="B46" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="E45" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
+      <c r="C46" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="D46" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="E46" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="C46" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="D46" s="6" t="s">
+      <c r="B47" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="E46" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="6" t="s">
+      <c r="C47" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="D47" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="E47" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="C47" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="D47" s="6" t="s">
+      <c r="B48" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="E47" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
+      <c r="C48" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="D48" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="E48" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="C48" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="D48" s="6" t="s">
+      <c r="B49" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="E48" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
+      <c r="C49" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="D49" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="E49" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="C49" s="6" t="s">
-        <v>295</v>
-      </c>
-      <c r="D49" s="6" t="s">
+      <c r="B50" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="E49" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
+      <c r="C50" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="D50" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="E50" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="C50" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="D50" s="6" t="s">
+      <c r="B51" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="E50" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
+      <c r="C51" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="D51" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="E51" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="C51" s="6" t="s">
-        <v>301</v>
-      </c>
-      <c r="D51" s="6" t="s">
+      <c r="B52" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="E51" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
+      <c r="C52" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="D52" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="E52" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="6" t="s">
         <v>304</v>
       </c>
-      <c r="C52" s="6" t="s">
-        <v>304</v>
-      </c>
-      <c r="D52" s="6" t="s">
+      <c r="B53" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="E52" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
+      <c r="C53" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="D53" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="E53" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="C53" s="6" t="s">
-        <v>307</v>
-      </c>
-      <c r="D53" s="6" t="s">
+      <c r="B54" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="E53" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F53" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="6" t="s">
+      <c r="C54" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="D54" s="6" t="s">
         <v>309</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="E54" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="C54" s="6" t="s">
-        <v>310</v>
-      </c>
-      <c r="D54" s="6" t="s">
+      <c r="B55" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="E54" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="6" t="s">
+      <c r="C55" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="D55" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="E55" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="C55" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="D55" s="6" t="s">
+      <c r="B56" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="E55" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
+      <c r="C56" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="D56" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="E56" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="C56" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="D56" s="6" t="s">
+      <c r="B57" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="E56" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F56" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
+      <c r="C57" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="D57" s="6" t="s">
         <v>318</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="E57" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="C57" s="6" t="s">
-        <v>319</v>
-      </c>
-      <c r="D57" s="6" t="s">
+      <c r="B58" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="E57" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
+      <c r="C58" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="D58" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="B58" s="6" t="s">
+      <c r="E58" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="C58" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="D58" s="6" t="s">
+      <c r="B59" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="E58" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F58" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
+      <c r="C59" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="D59" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="B59" s="6" t="s">
+      <c r="E59" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="C59" s="6" t="s">
-        <v>325</v>
-      </c>
-      <c r="D59" s="6" t="s">
+      <c r="B60" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="E59" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F59" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="6" t="s">
+      <c r="C60" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="D60" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="E60" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="C60" s="6" t="s">
-        <v>328</v>
-      </c>
-      <c r="D60" s="6" t="s">
+      <c r="B61" s="6" t="s">
         <v>329</v>
       </c>
-      <c r="E60" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F60" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
+      <c r="C61" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="D61" s="6" t="s">
         <v>330</v>
       </c>
-      <c r="B61" s="6" t="s">
+      <c r="E61" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="C61" s="6" t="s">
-        <v>331</v>
-      </c>
-      <c r="D61" s="6" t="s">
+      <c r="B62" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="E61" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F61" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="6" t="s">
+      <c r="C62" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="D62" s="6" t="s">
         <v>333</v>
       </c>
-      <c r="B62" s="6" t="s">
+      <c r="E62" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="C62" s="6" t="s">
-        <v>334</v>
-      </c>
-      <c r="D62" s="6" t="s">
+      <c r="B63" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="E62" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F62" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="6" t="s">
+      <c r="C63" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="D63" s="6" t="s">
         <v>336</v>
       </c>
-      <c r="B63" s="6" t="s">
-        <v>337</v>
-      </c>
-      <c r="C63" s="6" t="s">
-        <v>337</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>338</v>
-      </c>
       <c r="E63" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F63" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -3565,14 +3565,14 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="100.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="101.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="100.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="101.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3583,21 +3583,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>94</v>
       </c>
       <c r="C3" s="4"/>
     </row>
@@ -3614,14 +3614,14 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" customWidth="1"/>
-    <col min="2" max="2" width="210.7109375" customWidth="1"/>
-    <col min="3" max="3" width="129.85546875" customWidth="1"/>
+    <col min="1" max="1" width="35.5" customWidth="1"/>
+    <col min="2" max="2" width="210.6640625" customWidth="1"/>
+    <col min="3" max="3" width="129.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3632,109 +3632,109 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8" t="s">
+        <v>358</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:3" ht="112" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
         <v>359</v>
       </c>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B16" s="33" t="s">
         <v>360</v>
       </c>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
         <v>361</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="33" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -3751,18 +3751,18 @@
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.28515625" customWidth="1"/>
-    <col min="2" max="2" width="61.85546875" customWidth="1"/>
+    <col min="1" max="1" width="38.33203125" customWidth="1"/>
+    <col min="2" max="2" width="61.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -3778,70 +3778,70 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="73.85546875" customWidth="1"/>
+    <col min="1" max="1" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.83203125" customWidth="1"/>
     <col min="3" max="5" width="73" customWidth="1"/>
-    <col min="6" max="6" width="59.7109375" customWidth="1"/>
+    <col min="6" max="6" width="59.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="C2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>337</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>339</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>338</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>340</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -3857,59 +3857,59 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="64.42578125" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
-    <col min="8" max="9" width="48.5703125" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.42578125" customWidth="1"/>
-    <col min="12" max="12" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="64.5" customWidth="1"/>
+    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" customWidth="1"/>
+    <col min="8" max="9" width="48.5" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.5" customWidth="1"/>
+    <col min="12" max="12" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" customWidth="1"/>
-    <col min="15" max="15" width="108.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.1640625" customWidth="1"/>
+    <col min="15" max="15" width="108.5" bestFit="1" customWidth="1"/>
     <col min="16" max="18" width="77" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>9</v>
@@ -3924,13 +3924,13 @@
         <v>10</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="S1" s="3" t="s">
         <v>11</v>
@@ -3939,376 +3939,376 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B2" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="L2" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>38</v>
       </c>
       <c r="M2" s="7" t="s">
         <v>20</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O2" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P2" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Q2" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="R2" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="S2" s="6" t="s">
         <v>12</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O3" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P3" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Q3" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="R3" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="S3" s="6" t="s">
         <v>12</v>
       </c>
       <c r="T3" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L4" s="7" t="s">
         <v>16</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O4" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P4" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Q4" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="R4" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="S4" s="6" t="s">
         <v>12</v>
       </c>
       <c r="T4" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H5" s="26" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O5" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P5" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Q5" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="R5" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="S5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="T5" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G6" s="21" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H6" s="27" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="I6" s="21" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J6" s="22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K6" s="23" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="M6" s="20" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="N6" s="20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O6" s="24" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="P6" s="22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Q6" s="22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="R6" s="22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="S6" s="23" t="s">
         <v>12</v>
       </c>
       <c r="T6" s="20" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F7" s="20" t="b">
         <v>1</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H7" s="30" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K7" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="M7" s="20" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="N7" s="20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O7" s="24" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="Q7" s="26" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="S7" s="6" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="T7" s="20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -4334,7 +4334,7 @@
       <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4348,15 +4348,15 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="86.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="59.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="26.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="86.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="59.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4367,42 +4367,42 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:3" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4417,19 +4417,19 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.7109375" customWidth="1"/>
-    <col min="2" max="2" width="90.140625" customWidth="1"/>
-    <col min="3" max="3" width="108.28515625" customWidth="1"/>
+    <col min="1" max="1" width="45.6640625" customWidth="1"/>
+    <col min="2" max="2" width="90.1640625" customWidth="1"/>
+    <col min="3" max="3" width="108.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>7</v>

</xml_diff>